<commit_message>
initial baud gen module
</commit_message>
<xml_diff>
--- a/docs/reg_map.xlsx
+++ b/docs/reg_map.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="register_summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -221,6 +221,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -308,14 +309,15 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,18 +458,18 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="49.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updates for uart regfile
</commit_message>
<xml_diff>
--- a/docs/reg_map.xlsx
+++ b/docs/reg_map.xlsx
@@ -248,7 +248,7 @@
     <t xml:space="preserve">[15:0]</t>
   </si>
   <si>
-    <t xml:space="preserve">user</t>
+    <t xml:space="preserve">0x0029</t>
   </si>
   <si>
     <t xml:space="preserve">Integer divisor</t>
@@ -431,7 +431,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -485,17 +485,17 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.75"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Creation of tx and rx modules, work on top tb, work on integrating all modules in uart_top
</commit_message>
<xml_diff>
--- a/docs/reg_map.xlsx
+++ b/docs/reg_map.xlsx
@@ -152,7 +152,7 @@
     <t xml:space="preserve">RX_LVL</t>
   </si>
   <si>
-    <t xml:space="preserve">[5:2]</t>
+    <t xml:space="preserve">[6:2]</t>
   </si>
   <si>
     <t xml:space="preserve">RX FIFO occupancy</t>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">RX_BUSY</t>
   </si>
   <si>
-    <t xml:space="preserve">[6]</t>
+    <t xml:space="preserve">[7]</t>
   </si>
   <si>
     <t xml:space="preserve">RX engine active</t>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">TX_OVRN</t>
   </si>
   <si>
-    <t xml:space="preserve">[7]</t>
+    <t xml:space="preserve">[8]</t>
   </si>
   <si>
     <t xml:space="preserve">TX FIFO overrun</t>
@@ -179,7 +179,7 @@
     <t xml:space="preserve">TX_LVL</t>
   </si>
   <si>
-    <t xml:space="preserve">[11:8]</t>
+    <t xml:space="preserve">[13:9]</t>
   </si>
   <si>
     <t xml:space="preserve">TX FIFO occupancy</t>
@@ -188,13 +188,13 @@
     <t xml:space="preserve">TX_BUSY</t>
   </si>
   <si>
-    <t xml:space="preserve">[12]</t>
+    <t xml:space="preserve">[14]</t>
   </si>
   <si>
     <t xml:space="preserve">TX engine active</t>
   </si>
   <si>
-    <t xml:space="preserve">[31:13]</t>
+    <t xml:space="preserve">[31:15]</t>
   </si>
   <si>
     <t xml:space="preserve">0xC</t>
@@ -431,7 +431,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -485,10 +485,10 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>

</xml_diff>